<commit_message>
v3.0: BUGFIX Stunden-Berechnung, Analyse-Modul, Inactivity-Timeout
KRITISCHER BUGFIX:
- Monatstabelle und Kalender zeigen jetzt identische 'frei' Werte
- Beide nutzen Arbeitstage-Berechnung (ohne WE und Feiertage)
- Neue Funktion getWorkdaysInMonth()

ANALYSE-MODUL v5.11:
- Umbenennung Import → Analyse
- FZul Excel-Export mit Formatierung
- Feiertage bundesweit

SICHERHEIT:
- 30 Min Inactivity-Timeout
- sessionStorage statt localStorage

TYPESCRIPT-FIXES:
- Dashboard: Parameter-Typen ergänzt
- Import: Admin-Liste typisiert
</commit_message>
<xml_diff>
--- a/public/templates/FZul_Vorlage.xlsx
+++ b/public/templates/FZul_Vorlage.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdbs/Documents/Dev/projektzeiterfassung20/public/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF20CE6-462E-4946-9B8C-48506F1C10A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4445597-92E7-6A48-BC6D-765FE9C7DAD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-35300" yWindow="-28180" windowWidth="46320" windowHeight="28180" xr2:uid="{4E0623F2-5C98-4C26-BE2A-0325B7E83702}"/>
   </bookViews>
@@ -46,6 +46,378 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="131">
   <si>
+    <t>Wirtschaftsjahr:</t>
+  </si>
+  <si>
+    <t>Bundesland</t>
+  </si>
+  <si>
+    <t>Schleswig-Holstein</t>
+  </si>
+  <si>
+    <t>Angaben zum im FuE-Vorhaben unmittelbar mit FuE-Aktivitäten beschäftigten Arbeitnehmer:</t>
+  </si>
+  <si>
+    <t>Name:</t>
+  </si>
+  <si>
+    <t>Vorname:</t>
+  </si>
+  <si>
+    <t>Monat</t>
+  </si>
+  <si>
+    <t>Dokumentation der Arbeitsstunden für FuE-Tätigkeiten im FuE-Vorhaben</t>
+  </si>
+  <si>
+    <t>je Arbeitstag</t>
+  </si>
+  <si>
+    <t>FT</t>
+  </si>
+  <si>
+    <t>FT eff.</t>
+  </si>
+  <si>
+    <t>insg.</t>
+  </si>
+  <si>
+    <t>Bestätigung</t>
+  </si>
+  <si>
+    <t>Feiertage</t>
+  </si>
+  <si>
+    <t>Jahr</t>
+  </si>
+  <si>
+    <t>Untersschrift</t>
+  </si>
+  <si>
+    <t>Bayern</t>
+  </si>
+  <si>
+    <t>Datum</t>
+  </si>
+  <si>
+    <t>Abk.</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>WT</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>Frei</t>
+  </si>
+  <si>
+    <t>Neujahr</t>
+  </si>
+  <si>
+    <t>Neuj.</t>
+  </si>
+  <si>
+    <t>Hl. 3 Könige</t>
+  </si>
+  <si>
+    <t>Internat. Frauentag</t>
+  </si>
+  <si>
+    <t>Karfreitag</t>
+  </si>
+  <si>
+    <t>Karfr.</t>
+  </si>
+  <si>
+    <t>Ostersonntag</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>Ostermontag</t>
+  </si>
+  <si>
+    <t>OM</t>
+  </si>
+  <si>
+    <t>Tag der Arbeit</t>
+  </si>
+  <si>
+    <t>TdA</t>
+  </si>
+  <si>
+    <t>Christi Himmelfahrt</t>
+  </si>
+  <si>
+    <t>Chr.HF</t>
+  </si>
+  <si>
+    <t>Pfingstsonntag</t>
+  </si>
+  <si>
+    <t>PS</t>
+  </si>
+  <si>
+    <t>Pfingstmontag</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>Fronleichnam</t>
+  </si>
+  <si>
+    <t>Mariä Himmelfahrt</t>
+  </si>
+  <si>
+    <t>Tag der dt. Einheit</t>
+  </si>
+  <si>
+    <t>TDE</t>
+  </si>
+  <si>
+    <t>Reformationstag</t>
+  </si>
+  <si>
+    <t>Allerheiligen</t>
+  </si>
+  <si>
+    <t>1. Weihnachtstag</t>
+  </si>
+  <si>
+    <t>1.WT</t>
+  </si>
+  <si>
+    <t>2. Weihnachtstag</t>
+  </si>
+  <si>
+    <t>2.WT</t>
+  </si>
+  <si>
+    <t>Anzahl Feiertage</t>
+  </si>
+  <si>
+    <t>Summe der Arbeitsstunden für FuE-Tätigkeiten im FuE-Vorhaben:</t>
+  </si>
+  <si>
+    <t>wöchentliche Arbeitszeit:</t>
+  </si>
+  <si>
+    <t>Stunden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jahresarbeitsstunden (wöchentliche Arbeitszeit x 52 Wochen) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arbeitsvertraglich vereinbarter Urlaubsanspruch </t>
+  </si>
+  <si>
+    <t>Tage x</t>
+  </si>
+  <si>
+    <t>Stunden =</t>
+  </si>
+  <si>
+    <t>3K</t>
+  </si>
+  <si>
+    <t>IFT</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>MH</t>
+  </si>
+  <si>
+    <t>RT</t>
+  </si>
+  <si>
+    <t>AH</t>
+  </si>
+  <si>
+    <t>BB</t>
+  </si>
+  <si>
+    <t>Krankheitstage</t>
+  </si>
+  <si>
+    <t>Baden-Württemberg</t>
+  </si>
+  <si>
+    <t>BW</t>
+  </si>
+  <si>
+    <t>Sonderurlaub</t>
+  </si>
+  <si>
+    <t>BY</t>
+  </si>
+  <si>
+    <t>Gesetzliche Feiertage</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>Kurzarbeit, Erziehungsurlaub u. ä.</t>
+  </si>
+  <si>
+    <t>Brandenburg</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>Maßgebliche vereinbarte Jahresarbeitszeit</t>
+  </si>
+  <si>
+    <t>Bremen</t>
+  </si>
+  <si>
+    <t>HB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ggf. Kürzung auf Grund unterjährigem Beginn/Ende der FuE-Tätigkeit8 (x/12 x maßgebliche vereinbarte Jahresarbeitszeit) </t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>HH</t>
+  </si>
+  <si>
+    <t>Hessen</t>
+  </si>
+  <si>
+    <t>HE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Ermittlung des Anteils der Arbeitszeit für FuE-Tätigkeiten im FuE-Vorhaben </t>
+  </si>
+  <si>
+    <t>Mecklenburg-Vorpommern</t>
+  </si>
+  <si>
+    <t>MV</t>
+  </si>
+  <si>
+    <t>Niedersachsen</t>
+  </si>
+  <si>
+    <t>NI</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maßgebliche vereinbarte Jahresarbeitszeit (ggf. gekürzt) </t>
+  </si>
+  <si>
+    <t>Nordrhein-Westfalen</t>
+  </si>
+  <si>
+    <t>NW</t>
+  </si>
+  <si>
+    <t>Rheinland-Pfalz</t>
+  </si>
+  <si>
+    <t>RP</t>
+  </si>
+  <si>
+    <t>Saarland</t>
+  </si>
+  <si>
+    <t>SL</t>
+  </si>
+  <si>
+    <t>Zusätzlich bei Eigenforschung</t>
+  </si>
+  <si>
+    <t>Sachsen</t>
+  </si>
+  <si>
+    <t>SN</t>
+  </si>
+  <si>
+    <t>Sachsen-Anhalt</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Höchstgrenze12: x/12 x 2.080 Stunden </t>
+  </si>
+  <si>
+    <t>SH</t>
+  </si>
+  <si>
+    <t>Thüringen</t>
+  </si>
+  <si>
+    <t>TH</t>
+  </si>
+  <si>
+    <t>Gesehen und bestätigt:</t>
+  </si>
+  <si>
+    <t>Datum, Unterschrift (Arbeitnehmer)</t>
+  </si>
+  <si>
+    <t>Datum, Unterschrift (Projektverantwortlicher)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Die zu führende Stundenaufzeichnung über FuE-Tätigkeiten in einem begünstigten FuE-Vorhaben verbleibt beim Anspruchsberechtigten der Forschungszulage. Die Aufzeichnung kann zu Nachweiszwecken vorgelegt werden.
+Ist ein Arbeitnehmer oder im Fall von Eigenleistungen der selbst forschende Einzel- oder Mitunternehmer in mehreren begünstigten FuE-Vorhaben tätig, ist für jedes FuE-Vorhaben eine Stundenaufzeichnung zu führen. </t>
+  </si>
+  <si>
+    <t>2 Diese Bezeichnung entspricht idealerweise der Kurzbezeichnung aus der Bescheinigung nach § 6 FZulG der Bescheinigungsstelle Forschungszulage (BSFZ).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 Aus der Bescheinigung nach § 6 FZulG der BSFZ (soweit vorhanden). </t>
+  </si>
+  <si>
+    <t>4 Tätigkeitsbereich des Arbeitnehmers (z. B. Laborant). Hierzu gehören keine Tätigkeiten, die nur mittelbar oder unterstützend dem FuE-Vorhaben dienen (z. B. Management, Verwaltung, Transport oder sonstige Dienstleistungen).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 Die Bestätigung soll durch einen Projektverantwortlichen oder eine sonstige vom Anspruchsberechtigten beauftragte Person erfolgen. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 Auf Basis der vertraglich, tariflich oder betrieblich vereinbarten Jahresarbeitszeit. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 Zur Ermittlung der maßgeblichen Jahresarbeitszeit sind die Jahresarbeitsstunden um den arbeitsvertraglich vereinbarten Anspruch auf Urlaub und um die Arbeitszeit zu kürzen, in der der Arbeitnehmer dem Arbeitgeber wegen
+Krankheit, Sonderurlaub oder aufgrund von gesetzlichen Feiertagen, die auf Arbeitstage/Werktage entfallen, nicht zur Verfügung stand. Zur Ermittlung der Arbeitszeit in Stunden, die auf diese Tage entfällt, ist die vereinbarte
+wöchentliche Arbeitszeit durch die vereinbarten Arbeitstage pro Woche zu teilen. Das gilt auch für Kurzarbeit, Elternzeit u. ä. </t>
+  </si>
+  <si>
+    <t>8 Wird eine FuE-Tätigkeit im Laufe eines Jahres begonnen oder beendet, ist dies entsprechend zu berücksichtigen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9 Übernahme der Summe aus der Dokumentation der Arbeitsstunden im FuE-Vorhaben. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 Max. 1. Dies gilt auch, wenn ein Arbeitnehmer in mehreren FuE-Vorhaben tätig ist und sich aus allen FuE-Vorhaben insgesamt aufgrund Überstunden ein Wert größer als 1 ergeben würde. Die Aufteilung der förderfähigen
+Aufwendung erfolgt in diesen Fällen nach dem Verhältnis der Arbeitszeiten in den jeweiligen FuE-Vorhaben. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 Übernahme der Summe aus der Dokumentation der Arbeitsstunden im FuE-Vorhaben. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 Für jede Arbeitswoche sind maximal 40 Stunden förderfähig, d. h. 52 Wochen x 40 Stunden. Aus Vereinfachungsgründen erfolgt die Ermittlung der Höchstgrenze auf Monatsbasis, soweit die FuE-Tätigkeit im gesamten Monat
+erbracht wurde. Wird eine FuE-Vorhaben im Laufe eines Monats begonnen oder beendet, ist dies entsprechend zu berücksichtigen. Die Höchstgrenze gilt auch insgesamt für alle FuE-Vorhaben, wenn der selbst forschende
+Einzelunternehmer oder Mitunternehmer in mehreren begünstigten FuE-Vorhaben tätig ist. </t>
+  </si>
+  <si>
     <r>
       <t>Steuerliche Förderung von Forschung und Entwicklung (FuE) – Stundenaufzeichnung für FuE-Tätigkeiten in einembegünstigten FuE-Vorhaben</t>
     </r>
@@ -92,9 +464,6 @@
     </r>
   </si>
   <si>
-    <t>Wirtschaftsjahr:</t>
-  </si>
-  <si>
     <r>
       <t>Vorhaben-ID des FuE-Vorhabens</t>
     </r>
@@ -123,21 +492,6 @@
     </r>
   </si>
   <si>
-    <t>Bundesland</t>
-  </si>
-  <si>
-    <t>Schleswig-Holstein</t>
-  </si>
-  <si>
-    <t>Angaben zum im FuE-Vorhaben unmittelbar mit FuE-Aktivitäten beschäftigten Arbeitnehmer:</t>
-  </si>
-  <si>
-    <t>Name:</t>
-  </si>
-  <si>
-    <t>Vorname:</t>
-  </si>
-  <si>
     <r>
       <t>Kurzbezeichnung der FuE-Tätigkeit</t>
     </r>
@@ -166,147 +520,6 @@
     </r>
   </si>
   <si>
-    <t>Monat</t>
-  </si>
-  <si>
-    <t>Dokumentation der Arbeitsstunden für FuE-Tätigkeiten im FuE-Vorhaben</t>
-  </si>
-  <si>
-    <t>je Arbeitstag</t>
-  </si>
-  <si>
-    <t>FT</t>
-  </si>
-  <si>
-    <t>FT eff.</t>
-  </si>
-  <si>
-    <t>insg.</t>
-  </si>
-  <si>
-    <t>Bestätigung</t>
-  </si>
-  <si>
-    <t>Feiertage</t>
-  </si>
-  <si>
-    <t>Jahr</t>
-  </si>
-  <si>
-    <t>Untersschrift</t>
-  </si>
-  <si>
-    <t>Bayern</t>
-  </si>
-  <si>
-    <t>Datum</t>
-  </si>
-  <si>
-    <t>Abk.</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>WT</t>
-  </si>
-  <si>
-    <t>Tag</t>
-  </si>
-  <si>
-    <t>Frei</t>
-  </si>
-  <si>
-    <t>Neujahr</t>
-  </si>
-  <si>
-    <t>Neuj.</t>
-  </si>
-  <si>
-    <t>Hl. 3 Könige</t>
-  </si>
-  <si>
-    <t>Internat. Frauentag</t>
-  </si>
-  <si>
-    <t>Karfreitag</t>
-  </si>
-  <si>
-    <t>Karfr.</t>
-  </si>
-  <si>
-    <t>Ostersonntag</t>
-  </si>
-  <si>
-    <t>OS</t>
-  </si>
-  <si>
-    <t>Ostermontag</t>
-  </si>
-  <si>
-    <t>OM</t>
-  </si>
-  <si>
-    <t>Tag der Arbeit</t>
-  </si>
-  <si>
-    <t>TdA</t>
-  </si>
-  <si>
-    <t>Christi Himmelfahrt</t>
-  </si>
-  <si>
-    <t>Chr.HF</t>
-  </si>
-  <si>
-    <t>Pfingstsonntag</t>
-  </si>
-  <si>
-    <t>PS</t>
-  </si>
-  <si>
-    <t>Pfingstmontag</t>
-  </si>
-  <si>
-    <t>PM</t>
-  </si>
-  <si>
-    <t>Fronleichnam</t>
-  </si>
-  <si>
-    <t>Mariä Himmelfahrt</t>
-  </si>
-  <si>
-    <t>Tag der dt. Einheit</t>
-  </si>
-  <si>
-    <t>TDE</t>
-  </si>
-  <si>
-    <t>Reformationstag</t>
-  </si>
-  <si>
-    <t>Allerheiligen</t>
-  </si>
-  <si>
-    <t>1. Weihnachtstag</t>
-  </si>
-  <si>
-    <t>1.WT</t>
-  </si>
-  <si>
-    <t>2. Weihnachtstag</t>
-  </si>
-  <si>
-    <t>2.WT</t>
-  </si>
-  <si>
-    <t>Anzahl Feiertage</t>
-  </si>
-  <si>
-    <t>Summe der Arbeitsstunden für FuE-Tätigkeiten im FuE-Vorhaben:</t>
-  </si>
-  <si>
     <r>
       <t>1. Ermittlung der maßgeblichen vereinbarten Jahresarbeitszeit</t>
     </r>
@@ -324,15 +537,6 @@
     </r>
   </si>
   <si>
-    <t>wöchentliche Arbeitszeit:</t>
-  </si>
-  <si>
-    <t>Stunden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jahresarbeitsstunden (wöchentliche Arbeitszeit x 52 Wochen) </t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Abzgl. </t>
     </r>
@@ -349,102 +553,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Arbeitsvertraglich vereinbarter Urlaubsanspruch </t>
-  </si>
-  <si>
-    <t>Tage x</t>
-  </si>
-  <si>
-    <t>Stunden =</t>
-  </si>
-  <si>
-    <t>3K</t>
-  </si>
-  <si>
-    <t>IFT</t>
-  </si>
-  <si>
-    <t>FL</t>
-  </si>
-  <si>
-    <t>MH</t>
-  </si>
-  <si>
-    <t>RT</t>
-  </si>
-  <si>
-    <t>AH</t>
-  </si>
-  <si>
-    <t>BB</t>
-  </si>
-  <si>
-    <t>Krankheitstage</t>
-  </si>
-  <si>
-    <t>Baden-Württemberg</t>
-  </si>
-  <si>
-    <t>BW</t>
-  </si>
-  <si>
-    <t>Sonderurlaub</t>
-  </si>
-  <si>
-    <t>BY</t>
-  </si>
-  <si>
-    <t>Gesetzliche Feiertage</t>
-  </si>
-  <si>
-    <t>Berlin</t>
-  </si>
-  <si>
-    <t>BE</t>
-  </si>
-  <si>
-    <t>Kurzarbeit, Erziehungsurlaub u. ä.</t>
-  </si>
-  <si>
-    <t>Brandenburg</t>
-  </si>
-  <si>
-    <t>=</t>
-  </si>
-  <si>
-    <t>Maßgebliche vereinbarte Jahresarbeitszeit</t>
-  </si>
-  <si>
-    <t>Bremen</t>
-  </si>
-  <si>
-    <t>HB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ggf. Kürzung auf Grund unterjährigem Beginn/Ende der FuE-Tätigkeit8 (x/12 x maßgebliche vereinbarte Jahresarbeitszeit) </t>
-  </si>
-  <si>
-    <t>Hamburg</t>
-  </si>
-  <si>
-    <t>HH</t>
-  </si>
-  <si>
-    <t>Hessen</t>
-  </si>
-  <si>
-    <t>HE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2. Ermittlung des Anteils der Arbeitszeit für FuE-Tätigkeiten im FuE-Vorhaben </t>
-  </si>
-  <si>
-    <t>Mecklenburg-Vorpommern</t>
-  </si>
-  <si>
-    <t>MV</t>
-  </si>
-  <si>
     <r>
       <t>Summe der Arbeitsstunden für FuE-Tätigkeiten</t>
     </r>
@@ -461,24 +569,6 @@
     </r>
   </si>
   <si>
-    <t>Niedersachsen</t>
-  </si>
-  <si>
-    <t>NI</t>
-  </si>
-  <si>
-    <t>/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maßgebliche vereinbarte Jahresarbeitszeit (ggf. gekürzt) </t>
-  </si>
-  <si>
-    <t>Nordrhein-Westfalen</t>
-  </si>
-  <si>
-    <t>NW</t>
-  </si>
-  <si>
     <r>
       <t>Anteil der Arbeitszeit für FuE-Tätigkeiten im FuE-Vorhaben</t>
     </r>
@@ -495,27 +585,6 @@
     </r>
   </si>
   <si>
-    <t>Rheinland-Pfalz</t>
-  </si>
-  <si>
-    <t>RP</t>
-  </si>
-  <si>
-    <t>Saarland</t>
-  </si>
-  <si>
-    <t>SL</t>
-  </si>
-  <si>
-    <t>Zusätzlich bei Eigenforschung</t>
-  </si>
-  <si>
-    <t>Sachsen</t>
-  </si>
-  <si>
-    <t>SN</t>
-  </si>
-  <si>
     <r>
       <t>förderfähige Arbeitsstunden im begünstigten FuE-Vorhaben insgesamt</t>
     </r>
@@ -531,75 +600,6 @@
       <t>11</t>
     </r>
   </si>
-  <si>
-    <t>Sachsen-Anhalt</t>
-  </si>
-  <si>
-    <t>ST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Höchstgrenze12: x/12 x 2.080 Stunden </t>
-  </si>
-  <si>
-    <t>SH</t>
-  </si>
-  <si>
-    <t>Thüringen</t>
-  </si>
-  <si>
-    <t>TH</t>
-  </si>
-  <si>
-    <t>Gesehen und bestätigt:</t>
-  </si>
-  <si>
-    <t>Datum, Unterschrift (Arbeitnehmer)</t>
-  </si>
-  <si>
-    <t>Datum, Unterschrift (Projektverantwortlicher)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 Die zu führende Stundenaufzeichnung über FuE-Tätigkeiten in einem begünstigten FuE-Vorhaben verbleibt beim Anspruchsberechtigten der Forschungszulage. Die Aufzeichnung kann zu Nachweiszwecken vorgelegt werden.
-Ist ein Arbeitnehmer oder im Fall von Eigenleistungen der selbst forschende Einzel- oder Mitunternehmer in mehreren begünstigten FuE-Vorhaben tätig, ist für jedes FuE-Vorhaben eine Stundenaufzeichnung zu führen. </t>
-  </si>
-  <si>
-    <t>2 Diese Bezeichnung entspricht idealerweise der Kurzbezeichnung aus der Bescheinigung nach § 6 FZulG der Bescheinigungsstelle Forschungszulage (BSFZ).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 Aus der Bescheinigung nach § 6 FZulG der BSFZ (soweit vorhanden). </t>
-  </si>
-  <si>
-    <t>4 Tätigkeitsbereich des Arbeitnehmers (z. B. Laborant). Hierzu gehören keine Tätigkeiten, die nur mittelbar oder unterstützend dem FuE-Vorhaben dienen (z. B. Management, Verwaltung, Transport oder sonstige Dienstleistungen).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 Die Bestätigung soll durch einen Projektverantwortlichen oder eine sonstige vom Anspruchsberechtigten beauftragte Person erfolgen. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 Auf Basis der vertraglich, tariflich oder betrieblich vereinbarten Jahresarbeitszeit. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">7 Zur Ermittlung der maßgeblichen Jahresarbeitszeit sind die Jahresarbeitsstunden um den arbeitsvertraglich vereinbarten Anspruch auf Urlaub und um die Arbeitszeit zu kürzen, in der der Arbeitnehmer dem Arbeitgeber wegen
-Krankheit, Sonderurlaub oder aufgrund von gesetzlichen Feiertagen, die auf Arbeitstage/Werktage entfallen, nicht zur Verfügung stand. Zur Ermittlung der Arbeitszeit in Stunden, die auf diese Tage entfällt, ist die vereinbarte
-wöchentliche Arbeitszeit durch die vereinbarten Arbeitstage pro Woche zu teilen. Das gilt auch für Kurzarbeit, Elternzeit u. ä. </t>
-  </si>
-  <si>
-    <t>8 Wird eine FuE-Tätigkeit im Laufe eines Jahres begonnen oder beendet, ist dies entsprechend zu berücksichtigen.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9 Übernahme der Summe aus der Dokumentation der Arbeitsstunden im FuE-Vorhaben. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">10 Max. 1. Dies gilt auch, wenn ein Arbeitnehmer in mehreren FuE-Vorhaben tätig ist und sich aus allen FuE-Vorhaben insgesamt aufgrund Überstunden ein Wert größer als 1 ergeben würde. Die Aufteilung der förderfähigen
-Aufwendung erfolgt in diesen Fällen nach dem Verhältnis der Arbeitszeiten in den jeweiligen FuE-Vorhaben. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">11 Übernahme der Summe aus der Dokumentation der Arbeitsstunden im FuE-Vorhaben. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">12 Für jede Arbeitswoche sind maximal 40 Stunden förderfähig, d. h. 52 Wochen x 40 Stunden. Aus Vereinfachungsgründen erfolgt die Ermittlung der Höchstgrenze auf Monatsbasis, soweit die FuE-Tätigkeit im gesamten Monat
-erbracht wurde. Wird eine FuE-Vorhaben im Laufe eines Monats begonnen oder beendet, ist dies entsprechend zu berücksichtigen. Die Höchstgrenze gilt auch insgesamt für alle FuE-Vorhaben, wenn der selbst forschende
-Einzelunternehmer oder Mitunternehmer in mehreren begünstigten FuE-Vorhaben tätig ist. </t>
-  </si>
 </sst>
 </file>
 
@@ -611,7 +611,7 @@
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -733,8 +733,93 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -771,8 +856,200 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="55">
+  <borders count="87">
     <border>
       <left/>
       <right/>
@@ -1452,11 +1729,331 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="189">
+  <cellXfs count="219">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1920,12 +2517,132 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="33" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="34" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="35" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="36" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="37" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="38" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2745,20 +3462,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59F32849-35B7-43A1-8884-015D1999C0D1}">
-  <sheetPr>
+  <sheetPr codeName="Tabelle1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:BB76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33:AE33"/>
+      <selection activeCell="BF31" sqref="BF31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="32" width="4" customWidth="1"/>
-    <col min="33" max="33" width="7.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="23" customWidth="1"/>
     <col min="35" max="35" width="11.5" collapsed="1"/>
     <col min="36" max="36" width="11.5" hidden="1" customWidth="1" outlineLevel="1"/>
@@ -2783,7 +3500,7 @@
   <sheetData>
     <row r="1" spans="1:52" s="2" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="160" t="s">
-        <v>0</v>
+        <v>122</v>
       </c>
       <c r="B1" s="160"/>
       <c r="C1" s="160"/>
@@ -2873,45 +3590,45 @@
       <c r="AW2" s="37"/>
     </row>
     <row r="3" spans="1:52" s="2" customFormat="1" ht="25.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="170" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="170"/>
-      <c r="C3" s="170"/>
-      <c r="D3" s="170"/>
-      <c r="E3" s="170"/>
-      <c r="F3" s="170"/>
-      <c r="G3" s="170"/>
-      <c r="H3" s="170"/>
+      <c r="A3" s="200" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" s="200"/>
+      <c r="C3" s="200"/>
+      <c r="D3" s="200"/>
+      <c r="E3" s="200"/>
+      <c r="F3" s="200"/>
+      <c r="G3" s="200"/>
+      <c r="H3" s="200"/>
       <c r="I3" s="161"/>
-      <c r="J3" s="161"/>
-      <c r="K3" s="161"/>
-      <c r="L3" s="161"/>
-      <c r="M3" s="161"/>
-      <c r="N3" s="161"/>
-      <c r="O3" s="161"/>
-      <c r="P3" s="161"/>
-      <c r="Q3" s="161"/>
-      <c r="R3" s="161"/>
-      <c r="S3" s="161"/>
-      <c r="T3" s="161"/>
-      <c r="U3" s="161"/>
-      <c r="V3" s="161"/>
-      <c r="W3" s="161"/>
-      <c r="X3" s="161"/>
-      <c r="Y3" s="163" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z3" s="163"/>
-      <c r="AA3" s="163"/>
-      <c r="AB3" s="163"/>
-      <c r="AC3" s="163"/>
-      <c r="AD3" s="169">
+      <c r="J3" s="162"/>
+      <c r="K3" s="163"/>
+      <c r="L3" s="164"/>
+      <c r="M3" s="165"/>
+      <c r="N3" s="166"/>
+      <c r="O3" s="167"/>
+      <c r="P3" s="168"/>
+      <c r="Q3" s="169"/>
+      <c r="R3" s="170"/>
+      <c r="S3" s="171"/>
+      <c r="T3" s="172"/>
+      <c r="U3" s="173"/>
+      <c r="V3" s="174"/>
+      <c r="W3" s="175"/>
+      <c r="X3" s="176"/>
+      <c r="Y3" s="193" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="193"/>
+      <c r="AA3" s="193"/>
+      <c r="AB3" s="193"/>
+      <c r="AC3" s="193"/>
+      <c r="AD3" s="199">
         <v>2020</v>
       </c>
-      <c r="AE3" s="169"/>
-      <c r="AF3" s="169"/>
-      <c r="AG3" s="169"/>
+      <c r="AE3" s="199"/>
+      <c r="AF3" s="199"/>
+      <c r="AG3" s="199"/>
       <c r="AH3" s="17">
         <f>IF((MOD(YEAR(A10),4)=0)-(MOD(YEAR(A10),100)=0)+(MOD(YEAR(A10),400)=0)=0,0,1)</f>
         <v>1</v>
@@ -2925,46 +3642,46 @@
       <c r="AW3" s="37"/>
     </row>
     <row r="4" spans="1:52" s="2" customFormat="1" ht="25.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="170" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="170"/>
-      <c r="C4" s="170"/>
-      <c r="D4" s="170"/>
-      <c r="E4" s="170"/>
-      <c r="F4" s="170"/>
-      <c r="G4" s="170"/>
-      <c r="H4" s="170"/>
-      <c r="I4" s="162"/>
-      <c r="J4" s="162"/>
-      <c r="K4" s="162"/>
-      <c r="L4" s="162"/>
-      <c r="M4" s="162"/>
-      <c r="N4" s="162"/>
-      <c r="O4" s="162"/>
-      <c r="P4" s="162"/>
-      <c r="Q4" s="162"/>
-      <c r="R4" s="162"/>
-      <c r="S4" s="162"/>
-      <c r="T4" s="162"/>
-      <c r="U4" s="162"/>
-      <c r="V4" s="162"/>
-      <c r="W4" s="162"/>
-      <c r="X4" s="162"/>
-      <c r="Y4" s="163" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z4" s="163"/>
-      <c r="AA4" s="163"/>
-      <c r="AB4" s="163"/>
-      <c r="AC4" s="163"/>
-      <c r="AD4" s="177" t="s">
-        <v>110</v>
-      </c>
-      <c r="AE4" s="177"/>
-      <c r="AF4" s="177"/>
-      <c r="AG4" s="177"/>
-      <c r="AH4" s="177"/>
+      <c r="A4" s="200" t="s">
+        <v>124</v>
+      </c>
+      <c r="B4" s="200"/>
+      <c r="C4" s="200"/>
+      <c r="D4" s="200"/>
+      <c r="E4" s="200"/>
+      <c r="F4" s="200"/>
+      <c r="G4" s="200"/>
+      <c r="H4" s="200"/>
+      <c r="I4" s="177"/>
+      <c r="J4" s="178"/>
+      <c r="K4" s="179"/>
+      <c r="L4" s="180"/>
+      <c r="M4" s="181"/>
+      <c r="N4" s="182"/>
+      <c r="O4" s="183"/>
+      <c r="P4" s="184"/>
+      <c r="Q4" s="185"/>
+      <c r="R4" s="186"/>
+      <c r="S4" s="187"/>
+      <c r="T4" s="188"/>
+      <c r="U4" s="189"/>
+      <c r="V4" s="190"/>
+      <c r="W4" s="191"/>
+      <c r="X4" s="192"/>
+      <c r="Y4" s="193" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="193"/>
+      <c r="AA4" s="193"/>
+      <c r="AB4" s="193"/>
+      <c r="AC4" s="193"/>
+      <c r="AD4" s="207" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE4" s="207"/>
+      <c r="AF4" s="207"/>
+      <c r="AG4" s="207"/>
+      <c r="AH4" s="207"/>
       <c r="AK4" s="37"/>
       <c r="AO4" s="37"/>
       <c r="AP4" s="37"/>
@@ -2974,42 +3691,42 @@
       <c r="AW4" s="37"/>
     </row>
     <row r="5" spans="1:52" s="2" customFormat="1" ht="25.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="164" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="164"/>
-      <c r="C5" s="164"/>
-      <c r="D5" s="164"/>
-      <c r="E5" s="164"/>
-      <c r="F5" s="164"/>
-      <c r="G5" s="164"/>
-      <c r="H5" s="164"/>
-      <c r="I5" s="164"/>
-      <c r="J5" s="164"/>
-      <c r="K5" s="164"/>
-      <c r="L5" s="164"/>
-      <c r="M5" s="164"/>
-      <c r="N5" s="164"/>
-      <c r="O5" s="164"/>
-      <c r="P5" s="164"/>
-      <c r="Q5" s="164"/>
-      <c r="R5" s="164"/>
-      <c r="S5" s="164"/>
-      <c r="T5" s="164"/>
-      <c r="U5" s="164"/>
-      <c r="V5" s="164"/>
-      <c r="W5" s="164"/>
-      <c r="X5" s="164"/>
-      <c r="Y5" s="164"/>
-      <c r="Z5" s="164"/>
-      <c r="AA5" s="164"/>
-      <c r="AB5" s="164"/>
-      <c r="AC5" s="164"/>
-      <c r="AD5" s="164"/>
-      <c r="AE5" s="164"/>
-      <c r="AF5" s="164"/>
-      <c r="AG5" s="164"/>
-      <c r="AH5" s="164"/>
+      <c r="A5" s="194" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="194"/>
+      <c r="C5" s="194"/>
+      <c r="D5" s="194"/>
+      <c r="E5" s="194"/>
+      <c r="F5" s="194"/>
+      <c r="G5" s="194"/>
+      <c r="H5" s="194"/>
+      <c r="I5" s="194"/>
+      <c r="J5" s="194"/>
+      <c r="K5" s="194"/>
+      <c r="L5" s="194"/>
+      <c r="M5" s="194"/>
+      <c r="N5" s="194"/>
+      <c r="O5" s="194"/>
+      <c r="P5" s="194"/>
+      <c r="Q5" s="194"/>
+      <c r="R5" s="194"/>
+      <c r="S5" s="194"/>
+      <c r="T5" s="194"/>
+      <c r="U5" s="194"/>
+      <c r="V5" s="194"/>
+      <c r="W5" s="194"/>
+      <c r="X5" s="194"/>
+      <c r="Y5" s="194"/>
+      <c r="Z5" s="194"/>
+      <c r="AA5" s="194"/>
+      <c r="AB5" s="194"/>
+      <c r="AC5" s="194"/>
+      <c r="AD5" s="194"/>
+      <c r="AE5" s="194"/>
+      <c r="AF5" s="194"/>
+      <c r="AG5" s="194"/>
+      <c r="AH5" s="194"/>
       <c r="AK5" s="37"/>
       <c r="AO5" s="37"/>
       <c r="AP5" s="37"/>
@@ -3021,45 +3738,45 @@
     </row>
     <row r="6" spans="1:52" s="2" customFormat="1" ht="25.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="36" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="171"/>
-      <c r="C6" s="171"/>
-      <c r="D6" s="171"/>
-      <c r="E6" s="171"/>
-      <c r="F6" s="171"/>
-      <c r="G6" s="171"/>
-      <c r="H6" s="171"/>
-      <c r="I6" s="171"/>
-      <c r="J6" s="163" t="s">
-        <v>8</v>
-      </c>
-      <c r="K6" s="163"/>
-      <c r="L6" s="163"/>
-      <c r="M6" s="171"/>
-      <c r="N6" s="171"/>
-      <c r="O6" s="171"/>
-      <c r="P6" s="171"/>
-      <c r="Q6" s="171"/>
-      <c r="R6" s="171"/>
-      <c r="S6" s="171"/>
-      <c r="T6" s="171"/>
-      <c r="U6" s="163" t="s">
-        <v>9</v>
-      </c>
-      <c r="V6" s="163"/>
-      <c r="W6" s="163"/>
-      <c r="X6" s="163"/>
-      <c r="Y6" s="163"/>
-      <c r="Z6" s="163"/>
-      <c r="AA6" s="163"/>
-      <c r="AB6" s="163"/>
-      <c r="AC6" s="163"/>
-      <c r="AD6" s="171"/>
-      <c r="AE6" s="171"/>
-      <c r="AF6" s="171"/>
-      <c r="AG6" s="171"/>
-      <c r="AH6" s="171"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="201"/>
+      <c r="C6" s="201"/>
+      <c r="D6" s="201"/>
+      <c r="E6" s="201"/>
+      <c r="F6" s="201"/>
+      <c r="G6" s="201"/>
+      <c r="H6" s="201"/>
+      <c r="I6" s="201"/>
+      <c r="J6" s="193" t="s">
+        <v>5</v>
+      </c>
+      <c r="K6" s="193"/>
+      <c r="L6" s="193"/>
+      <c r="M6" s="201"/>
+      <c r="N6" s="201"/>
+      <c r="O6" s="201"/>
+      <c r="P6" s="201"/>
+      <c r="Q6" s="201"/>
+      <c r="R6" s="201"/>
+      <c r="S6" s="201"/>
+      <c r="T6" s="201"/>
+      <c r="U6" s="193" t="s">
+        <v>125</v>
+      </c>
+      <c r="V6" s="193"/>
+      <c r="W6" s="193"/>
+      <c r="X6" s="193"/>
+      <c r="Y6" s="193"/>
+      <c r="Z6" s="193"/>
+      <c r="AA6" s="193"/>
+      <c r="AB6" s="193"/>
+      <c r="AC6" s="193"/>
+      <c r="AD6" s="201"/>
+      <c r="AE6" s="201"/>
+      <c r="AF6" s="201"/>
+      <c r="AG6" s="201"/>
+      <c r="AH6" s="201"/>
       <c r="AK6" s="37"/>
       <c r="AO6" s="37"/>
       <c r="AP6" s="37"/>
@@ -3069,42 +3786,42 @@
       <c r="AW6" s="37"/>
     </row>
     <row r="7" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="172" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="176" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="176"/>
-      <c r="D7" s="176"/>
-      <c r="E7" s="176"/>
-      <c r="F7" s="176"/>
-      <c r="G7" s="176"/>
-      <c r="H7" s="176"/>
-      <c r="I7" s="176"/>
-      <c r="J7" s="176"/>
-      <c r="K7" s="176"/>
-      <c r="L7" s="176"/>
-      <c r="M7" s="176"/>
-      <c r="N7" s="176"/>
-      <c r="O7" s="176"/>
-      <c r="P7" s="176"/>
-      <c r="Q7" s="176"/>
-      <c r="R7" s="176"/>
-      <c r="S7" s="176"/>
-      <c r="T7" s="176"/>
-      <c r="U7" s="176"/>
-      <c r="V7" s="176"/>
-      <c r="W7" s="176"/>
-      <c r="X7" s="176"/>
-      <c r="Y7" s="176"/>
-      <c r="Z7" s="176"/>
-      <c r="AA7" s="176"/>
-      <c r="AB7" s="176"/>
-      <c r="AC7" s="176"/>
-      <c r="AD7" s="176"/>
-      <c r="AE7" s="176"/>
-      <c r="AF7" s="176"/>
+      <c r="A7" s="202" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="206" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="206"/>
+      <c r="D7" s="206"/>
+      <c r="E7" s="206"/>
+      <c r="F7" s="206"/>
+      <c r="G7" s="206"/>
+      <c r="H7" s="206"/>
+      <c r="I7" s="206"/>
+      <c r="J7" s="206"/>
+      <c r="K7" s="206"/>
+      <c r="L7" s="206"/>
+      <c r="M7" s="206"/>
+      <c r="N7" s="206"/>
+      <c r="O7" s="206"/>
+      <c r="P7" s="206"/>
+      <c r="Q7" s="206"/>
+      <c r="R7" s="206"/>
+      <c r="S7" s="206"/>
+      <c r="T7" s="206"/>
+      <c r="U7" s="206"/>
+      <c r="V7" s="206"/>
+      <c r="W7" s="206"/>
+      <c r="X7" s="206"/>
+      <c r="Y7" s="206"/>
+      <c r="Z7" s="206"/>
+      <c r="AA7" s="206"/>
+      <c r="AB7" s="206"/>
+      <c r="AC7" s="206"/>
+      <c r="AD7" s="206"/>
+      <c r="AE7" s="206"/>
+      <c r="AF7" s="206"/>
       <c r="AG7" s="14"/>
       <c r="AH7" s="5"/>
       <c r="AI7"/>
@@ -3117,56 +3834,56 @@
       <c r="AR7" s="37"/>
       <c r="AZ7" s="37" t="str">
         <f>VLOOKUP($AD$4,$AS$40:$AT$55,2)</f>
-        <v>ST</v>
+        <v>BY</v>
       </c>
     </row>
     <row r="8" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A8" s="173"/>
-      <c r="B8" s="175" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="175"/>
-      <c r="D8" s="175"/>
-      <c r="E8" s="175"/>
-      <c r="F8" s="175"/>
-      <c r="G8" s="175"/>
-      <c r="H8" s="175"/>
-      <c r="I8" s="175"/>
-      <c r="J8" s="175"/>
-      <c r="K8" s="175"/>
-      <c r="L8" s="175"/>
-      <c r="M8" s="175"/>
-      <c r="N8" s="175"/>
-      <c r="O8" s="175"/>
-      <c r="P8" s="175"/>
-      <c r="Q8" s="175"/>
-      <c r="R8" s="175"/>
-      <c r="S8" s="175"/>
-      <c r="T8" s="175"/>
-      <c r="U8" s="175"/>
-      <c r="V8" s="175"/>
-      <c r="W8" s="175"/>
-      <c r="X8" s="175"/>
-      <c r="Y8" s="175"/>
-      <c r="Z8" s="175"/>
-      <c r="AA8" s="175"/>
-      <c r="AB8" s="175"/>
-      <c r="AC8" s="175"/>
-      <c r="AD8" s="175"/>
-      <c r="AE8" s="175"/>
-      <c r="AF8" s="175"/>
+      <c r="A8" s="203"/>
+      <c r="B8" s="205" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="205"/>
+      <c r="D8" s="205"/>
+      <c r="E8" s="205"/>
+      <c r="F8" s="205"/>
+      <c r="G8" s="205"/>
+      <c r="H8" s="205"/>
+      <c r="I8" s="205"/>
+      <c r="J8" s="205"/>
+      <c r="K8" s="205"/>
+      <c r="L8" s="205"/>
+      <c r="M8" s="205"/>
+      <c r="N8" s="205"/>
+      <c r="O8" s="205"/>
+      <c r="P8" s="205"/>
+      <c r="Q8" s="205"/>
+      <c r="R8" s="205"/>
+      <c r="S8" s="205"/>
+      <c r="T8" s="205"/>
+      <c r="U8" s="205"/>
+      <c r="V8" s="205"/>
+      <c r="W8" s="205"/>
+      <c r="X8" s="205"/>
+      <c r="Y8" s="205"/>
+      <c r="Z8" s="205"/>
+      <c r="AA8" s="205"/>
+      <c r="AB8" s="205"/>
+      <c r="AC8" s="205"/>
+      <c r="AD8" s="205"/>
+      <c r="AE8" s="205"/>
+      <c r="AF8" s="205"/>
       <c r="AG8" s="15"/>
       <c r="AH8" s="6"/>
-      <c r="AK8" s="185" t="s">
-        <v>13</v>
-      </c>
-      <c r="AL8" s="185" t="s">
-        <v>14</v>
+      <c r="AK8" s="215" t="s">
+        <v>9</v>
+      </c>
+      <c r="AL8" s="215" t="s">
+        <v>10</v>
       </c>
       <c r="AM8" s="71"/>
     </row>
     <row r="9" spans="1:52" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="174"/>
+      <c r="A9" s="204"/>
       <c r="B9" s="3">
         <v>1</v>
       </c>
@@ -3261,18 +3978,18 @@
         <v>31</v>
       </c>
       <c r="AG9" s="16" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="AH9" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="AK9" s="185"/>
-      <c r="AL9" s="185"/>
+        <v>12</v>
+      </c>
+      <c r="AK9" s="215"/>
+      <c r="AL9" s="215"/>
       <c r="AM9" s="71"/>
       <c r="AT9" s="2"/>
     </row>
     <row r="10" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A10" s="166">
+      <c r="A10" s="196">
         <f>DATE($AD$3,1,1)</f>
         <v>43831</v>
       </c>
@@ -3400,7 +4117,7 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="AG10" s="165">
+      <c r="AG10" s="195">
         <f>SUM(B11:AF11)</f>
         <v>0</v>
       </c>
@@ -3419,13 +4136,13 @@
       </c>
       <c r="AT10" s="37"/>
       <c r="AU10" s="47" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="AV10" s="59"/>
-      <c r="AW10" s="178" t="s">
-        <v>18</v>
-      </c>
-      <c r="AX10" s="178"/>
+      <c r="AW10" s="208" t="s">
+        <v>14</v>
+      </c>
+      <c r="AX10" s="208"/>
       <c r="AY10" s="60"/>
       <c r="AZ10" s="61">
         <f>$AD$3</f>
@@ -3433,7 +4150,7 @@
       </c>
     </row>
     <row r="11" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A11" s="166"/>
+      <c r="A11" s="196"/>
       <c r="B11" s="51"/>
       <c r="C11" s="50"/>
       <c r="D11" s="50"/>
@@ -3465,24 +4182,24 @@
       <c r="AD11" s="50"/>
       <c r="AE11" s="50"/>
       <c r="AF11" s="50"/>
-      <c r="AG11" s="165"/>
+      <c r="AG11" s="195"/>
       <c r="AH11" s="9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="AT11" s="37"/>
       <c r="AU11" s="43" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="AV11" s="1"/>
-      <c r="AW11" s="188" t="s">
-        <v>21</v>
-      </c>
-      <c r="AX11" s="188"/>
+      <c r="AW11" s="218" t="s">
+        <v>17</v>
+      </c>
+      <c r="AX11" s="218"/>
       <c r="AY11" s="1"/>
       <c r="AZ11" s="44"/>
     </row>
     <row r="12" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A12" s="166">
+      <c r="A12" s="196">
         <f>EOMONTH(A10,0)+1</f>
         <v>43862</v>
       </c>
@@ -3602,9 +4319,9 @@
         <f t="shared" ref="AD12" si="2">WEEKDAY(DATE($AD$3,MONTH($A12),AD$9))</f>
         <v>7</v>
       </c>
-      <c r="AE12" s="168"/>
-      <c r="AF12" s="168"/>
-      <c r="AG12" s="165">
+      <c r="AE12" s="198"/>
+      <c r="AF12" s="198"/>
+      <c r="AG12" s="195">
         <f>SUM(B13:AF13)</f>
         <v>0</v>
       </c>
@@ -3622,38 +4339,38 @@
         <v>0</v>
       </c>
       <c r="AN12" s="65" t="s">
+        <v>13</v>
+      </c>
+      <c r="AO12" s="66" t="s">
+        <v>18</v>
+      </c>
+      <c r="AP12" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="AO12" s="66" t="s">
-        <v>22</v>
-      </c>
-      <c r="AP12" s="66" t="s">
-        <v>21</v>
-      </c>
       <c r="AQ12" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="AR12" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="AT12" s="37"/>
       <c r="AU12" s="56"/>
       <c r="AV12" s="57"/>
       <c r="AW12" s="57" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="AX12" s="57" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="AY12" s="57" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="AZ12" s="58" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A13" s="167"/>
+      <c r="A13" s="197"/>
       <c r="B13" s="50"/>
       <c r="C13" s="50"/>
       <c r="D13" s="50"/>
@@ -3683,11 +4400,11 @@
       <c r="AB13" s="50"/>
       <c r="AC13" s="50"/>
       <c r="AD13" s="50"/>
-      <c r="AE13" s="168"/>
-      <c r="AF13" s="168"/>
-      <c r="AG13" s="165"/>
+      <c r="AE13" s="198"/>
+      <c r="AF13" s="198"/>
+      <c r="AG13" s="195"/>
       <c r="AH13" s="9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="AN13" s="63" t="str">
         <f t="shared" ref="AN13:AN27" si="3">AU13</f>
@@ -3714,10 +4431,10 @@
         <v>43831</v>
       </c>
       <c r="AU13" s="48" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="AV13" s="40" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="AW13" s="40">
         <v>1</v>
@@ -3735,7 +4452,7 @@
       </c>
     </row>
     <row r="14" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A14" s="166">
+      <c r="A14" s="196">
         <f>EOMONTH(A12,0)+1</f>
         <v>43891</v>
       </c>
@@ -3863,7 +4580,7 @@
         <f t="shared" si="8"/>
         <v>3</v>
       </c>
-      <c r="AG14" s="165">
+      <c r="AG14" s="195">
         <f t="shared" ref="AG14" si="9">SUM(B15:AF15)</f>
         <v>0</v>
       </c>
@@ -3905,7 +4622,7 @@
         <v>43836</v>
       </c>
       <c r="AU14" s="49" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="AV14" s="41" t="str">
         <f>IF(AZ14=0,AY14,"Hl.3K")</f>
@@ -3927,7 +4644,7 @@
       </c>
     </row>
     <row r="15" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A15" s="167"/>
+      <c r="A15" s="197"/>
       <c r="B15" s="50"/>
       <c r="C15" s="50"/>
       <c r="D15" s="50"/>
@@ -3959,9 +4676,9 @@
       <c r="AD15" s="50"/>
       <c r="AE15" s="50"/>
       <c r="AF15" s="50"/>
-      <c r="AG15" s="165"/>
+      <c r="AG15" s="195"/>
       <c r="AH15" s="9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="AN15" s="63" t="str">
         <f t="shared" si="3"/>
@@ -3988,7 +4705,7 @@
         <v>43898</v>
       </c>
       <c r="AU15" s="49" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="AV15" s="41">
         <f>IF(AZ15=0,AY15,"IFT")</f>
@@ -4010,7 +4727,7 @@
       </c>
     </row>
     <row r="16" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A16" s="166">
+      <c r="A16" s="196">
         <f t="shared" ref="A16" si="11">EOMONTH(A14,0)+1</f>
         <v>43922</v>
       </c>
@@ -4134,8 +4851,8 @@
         <f t="shared" si="12"/>
         <v>5</v>
       </c>
-      <c r="AF16" s="168"/>
-      <c r="AG16" s="165">
+      <c r="AF16" s="198"/>
+      <c r="AG16" s="195">
         <f t="shared" ref="AG16" si="13">SUM(B17:AF17)</f>
         <v>0</v>
       </c>
@@ -4177,10 +4894,10 @@
         <v>43931</v>
       </c>
       <c r="AU16" s="49" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="AV16" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="AW16" s="1">
         <f>AW17</f>
@@ -4200,7 +4917,7 @@
       </c>
     </row>
     <row r="17" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A17" s="167"/>
+      <c r="A17" s="197"/>
       <c r="B17" s="50"/>
       <c r="C17" s="50"/>
       <c r="D17" s="50"/>
@@ -4231,10 +4948,10 @@
       <c r="AC17" s="50"/>
       <c r="AD17" s="50"/>
       <c r="AE17" s="50"/>
-      <c r="AF17" s="168"/>
-      <c r="AG17" s="165"/>
+      <c r="AF17" s="198"/>
+      <c r="AG17" s="195"/>
       <c r="AH17" s="9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="AN17" s="63" t="str">
         <f t="shared" si="3"/>
@@ -4261,10 +4978,10 @@
         <v>43933</v>
       </c>
       <c r="AU17" s="49" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="AV17" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="AW17" s="1">
         <f>MONTH(AT17)</f>
@@ -4284,7 +5001,7 @@
       </c>
     </row>
     <row r="18" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A18" s="166">
+      <c r="A18" s="196">
         <f t="shared" ref="A18" si="14">EOMONTH(A16,0)+1</f>
         <v>43952</v>
       </c>
@@ -4412,7 +5129,7 @@
         <f t="shared" si="15"/>
         <v>PS</v>
       </c>
-      <c r="AG18" s="165">
+      <c r="AG18" s="195">
         <f t="shared" ref="AG18" si="16">SUM(B19:AF19)</f>
         <v>0</v>
       </c>
@@ -4454,10 +5171,10 @@
         <v>43934</v>
       </c>
       <c r="AU18" s="49" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="AV18" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="AW18" s="1">
         <f>AW17</f>
@@ -4477,7 +5194,7 @@
       </c>
     </row>
     <row r="19" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A19" s="167"/>
+      <c r="A19" s="197"/>
       <c r="B19" s="50"/>
       <c r="C19" s="50"/>
       <c r="D19" s="50"/>
@@ -4509,9 +5226,9 @@
       <c r="AD19" s="50"/>
       <c r="AE19" s="50"/>
       <c r="AF19" s="50"/>
-      <c r="AG19" s="165"/>
+      <c r="AG19" s="195"/>
       <c r="AH19" s="9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="AN19" s="63" t="str">
         <f t="shared" si="3"/>
@@ -4538,10 +5255,10 @@
         <v>43952</v>
       </c>
       <c r="AU19" s="49" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="AV19" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="AW19" s="1">
         <v>5</v>
@@ -4559,7 +5276,7 @@
       </c>
     </row>
     <row r="20" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A20" s="166">
+      <c r="A20" s="196">
         <f t="shared" ref="A20" si="18">EOMONTH(A18,0)+1</f>
         <v>43983</v>
       </c>
@@ -4603,9 +5320,9 @@
         <f t="shared" si="19"/>
         <v>4</v>
       </c>
-      <c r="L20" s="52">
+      <c r="L20" s="52" t="str">
         <f t="shared" si="19"/>
-        <v>5</v>
+        <v>Fronl.</v>
       </c>
       <c r="M20" s="52">
         <f t="shared" si="19"/>
@@ -4683,8 +5400,8 @@
         <f t="shared" si="19"/>
         <v>3</v>
       </c>
-      <c r="AF20" s="168"/>
-      <c r="AG20" s="165">
+      <c r="AF20" s="198"/>
+      <c r="AG20" s="195">
         <f t="shared" ref="AG20" si="20">SUM(B21:AF21)</f>
         <v>0</v>
       </c>
@@ -4727,10 +5444,10 @@
         <v>43972</v>
       </c>
       <c r="AU20" s="49" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="AV20" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="AW20" s="1">
         <f>MONTH(AT20)</f>
@@ -4750,7 +5467,7 @@
       </c>
     </row>
     <row r="21" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A21" s="167"/>
+      <c r="A21" s="197"/>
       <c r="B21" s="50"/>
       <c r="C21" s="50"/>
       <c r="D21" s="50"/>
@@ -4781,10 +5498,10 @@
       <c r="AC21" s="50"/>
       <c r="AD21" s="50"/>
       <c r="AE21" s="50"/>
-      <c r="AF21" s="168"/>
-      <c r="AG21" s="165"/>
+      <c r="AF21" s="198"/>
+      <c r="AG21" s="195"/>
       <c r="AH21" s="9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="AN21" s="63" t="str">
         <f t="shared" si="3"/>
@@ -4811,10 +5528,10 @@
         <v>43982</v>
       </c>
       <c r="AU21" s="49" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="AV21" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="AW21" s="1">
         <f>MONTH(AT21)</f>
@@ -4834,7 +5551,7 @@
       </c>
     </row>
     <row r="22" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A22" s="166">
+      <c r="A22" s="196">
         <f t="shared" ref="A22" si="21">EOMONTH(A20,0)+1</f>
         <v>44013</v>
       </c>
@@ -4962,7 +5679,7 @@
         <f t="shared" si="22"/>
         <v>6</v>
       </c>
-      <c r="AG22" s="165">
+      <c r="AG22" s="195">
         <f t="shared" ref="AG22" si="23">SUM(B23:AF23)</f>
         <v>0</v>
       </c>
@@ -5004,10 +5721,10 @@
         <v>43983</v>
       </c>
       <c r="AU22" s="49" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="AV22" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="AW22" s="1">
         <f>AW21</f>
@@ -5027,7 +5744,7 @@
       </c>
     </row>
     <row r="23" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A23" s="167"/>
+      <c r="A23" s="197"/>
       <c r="B23" s="50"/>
       <c r="C23" s="50"/>
       <c r="D23" s="50"/>
@@ -5059,17 +5776,17 @@
       <c r="AD23" s="50"/>
       <c r="AE23" s="50"/>
       <c r="AF23" s="50"/>
-      <c r="AG23" s="165"/>
+      <c r="AG23" s="195"/>
       <c r="AH23" s="9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="AN23" s="63" t="str">
         <f t="shared" si="3"/>
         <v>Fronleichnam</v>
       </c>
-      <c r="AO23" s="64">
+      <c r="AO23" s="64" t="str">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>Fronl.</v>
       </c>
       <c r="AP23" s="67">
         <f t="shared" si="5"/>
@@ -5088,11 +5805,11 @@
         <v>43993</v>
       </c>
       <c r="AU23" s="49" t="s">
-        <v>45</v>
-      </c>
-      <c r="AV23" s="41">
+        <v>41</v>
+      </c>
+      <c r="AV23" s="41" t="str">
         <f>IF(AZ23=0,AY23,"Fronl.")</f>
-        <v>5</v>
+        <v>Fronl.</v>
       </c>
       <c r="AW23" s="1">
         <f>MONTH(AT23)</f>
@@ -5108,11 +5825,11 @@
       </c>
       <c r="AZ23" s="44">
         <f>IF(VLOOKUP($AZ$7,$AT$40:$BA$55,4,FALSE)=1,IF(WEEKDAY(DATE($AZ$10,AW23,AX23))=1,0,IF(WEEKDAY(DATE($AZ$10,AW23,AX23))=7,0,1)),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A24" s="166">
+      <c r="A24" s="196">
         <f t="shared" ref="A24" si="24">EOMONTH(A22,0)+1</f>
         <v>44044</v>
       </c>
@@ -5240,7 +5957,7 @@
         <f t="shared" si="25"/>
         <v>2</v>
       </c>
-      <c r="AG24" s="165">
+      <c r="AG24" s="195">
         <f t="shared" ref="AG24" si="26">SUM(B25:AF25)</f>
         <v>0</v>
       </c>
@@ -5282,7 +5999,7 @@
         <v>44058</v>
       </c>
       <c r="AU24" s="49" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="AV24" s="41">
         <f>IF(AZ24=0,AY24,"M.HF")</f>
@@ -5304,7 +6021,7 @@
       </c>
     </row>
     <row r="25" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A25" s="167"/>
+      <c r="A25" s="197"/>
       <c r="B25" s="50"/>
       <c r="C25" s="50"/>
       <c r="D25" s="50"/>
@@ -5336,9 +6053,9 @@
       <c r="AD25" s="50"/>
       <c r="AE25" s="50"/>
       <c r="AF25" s="50"/>
-      <c r="AG25" s="165"/>
+      <c r="AG25" s="195"/>
       <c r="AH25" s="9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="AN25" s="63" t="str">
         <f t="shared" si="3"/>
@@ -5365,10 +6082,10 @@
         <v>44107</v>
       </c>
       <c r="AU25" s="49" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="AV25" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="AW25" s="1">
         <v>10</v>
@@ -5386,7 +6103,7 @@
       </c>
     </row>
     <row r="26" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A26" s="166">
+      <c r="A26" s="196">
         <f t="shared" ref="A26" si="29">EOMONTH(A24,0)+1</f>
         <v>44075</v>
       </c>
@@ -5510,8 +6227,8 @@
         <f t="shared" si="30"/>
         <v>4</v>
       </c>
-      <c r="AF26" s="168"/>
-      <c r="AG26" s="165">
+      <c r="AF26" s="198"/>
+      <c r="AG26" s="195">
         <f t="shared" ref="AG26" si="31">SUM(B27:AF27)</f>
         <v>0</v>
       </c>
@@ -5553,7 +6270,7 @@
         <v>44135</v>
       </c>
       <c r="AU26" s="49" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="AV26" s="41">
         <f>IF(AZ26=0,AY26,"RT")</f>
@@ -5575,7 +6292,7 @@
       </c>
     </row>
     <row r="27" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A27" s="167"/>
+      <c r="A27" s="197"/>
       <c r="B27" s="50"/>
       <c r="C27" s="50"/>
       <c r="D27" s="50"/>
@@ -5606,10 +6323,10 @@
       <c r="AC27" s="50"/>
       <c r="AD27" s="50"/>
       <c r="AE27" s="50"/>
-      <c r="AF27" s="168"/>
-      <c r="AG27" s="165"/>
+      <c r="AF27" s="198"/>
+      <c r="AG27" s="195"/>
       <c r="AH27" s="9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="AN27" s="63" t="str">
         <f t="shared" si="3"/>
@@ -5636,7 +6353,7 @@
         <v>44136</v>
       </c>
       <c r="AU27" s="49" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="AV27" s="41">
         <f>IF(AZ27=0,AY27,"Allerh.")</f>
@@ -5658,7 +6375,7 @@
       </c>
     </row>
     <row r="28" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A28" s="166">
+      <c r="A28" s="196">
         <f t="shared" ref="A28" si="33">EOMONTH(A26,0)+1</f>
         <v>44105</v>
       </c>
@@ -5786,7 +6503,7 @@
         <f t="shared" si="34"/>
         <v>7</v>
       </c>
-      <c r="AG28" s="165">
+      <c r="AG28" s="195">
         <f t="shared" ref="AG28" si="35">SUM(B29:AF29)</f>
         <v>0</v>
       </c>
@@ -5828,10 +6545,10 @@
         <v>44190</v>
       </c>
       <c r="AU28" s="49" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="AV28" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="AW28" s="1">
         <v>12</v>
@@ -5849,7 +6566,7 @@
       </c>
     </row>
     <row r="29" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A29" s="167"/>
+      <c r="A29" s="197"/>
       <c r="B29" s="50"/>
       <c r="C29" s="50"/>
       <c r="D29" s="50"/>
@@ -5881,9 +6598,9 @@
       <c r="AD29" s="50"/>
       <c r="AE29" s="50"/>
       <c r="AF29" s="50"/>
-      <c r="AG29" s="165"/>
+      <c r="AG29" s="195"/>
       <c r="AH29" s="9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="AN29" s="63" t="str">
         <f>AU29</f>
@@ -5910,10 +6627,10 @@
         <v>44191</v>
       </c>
       <c r="AU29" s="49" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="AV29" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="AW29" s="1">
         <v>12</v>
@@ -5931,7 +6648,7 @@
       </c>
     </row>
     <row r="30" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A30" s="166">
+      <c r="A30" s="196">
         <f t="shared" ref="A30:A32" si="36">EOMONTH(A28,0)+1</f>
         <v>44136</v>
       </c>
@@ -6055,8 +6772,8 @@
         <f t="shared" si="37"/>
         <v>2</v>
       </c>
-      <c r="AF30" s="168"/>
-      <c r="AG30" s="165">
+      <c r="AF30" s="198"/>
+      <c r="AG30" s="195">
         <f t="shared" ref="AG30" si="38">SUM(B31:AF31)</f>
         <v>0</v>
       </c>
@@ -6078,20 +6795,20 @@
       <c r="AR30" s="54"/>
       <c r="AS30" s="38"/>
       <c r="AT30" s="37"/>
-      <c r="AU30" s="179" t="s">
-        <v>55</v>
-      </c>
-      <c r="AV30" s="180"/>
-      <c r="AW30" s="180"/>
-      <c r="AX30" s="180"/>
-      <c r="AY30" s="181"/>
-      <c r="AZ30" s="186">
+      <c r="AU30" s="209" t="s">
+        <v>51</v>
+      </c>
+      <c r="AV30" s="210"/>
+      <c r="AW30" s="210"/>
+      <c r="AX30" s="210"/>
+      <c r="AY30" s="211"/>
+      <c r="AZ30" s="216">
         <f>SUM(AZ13:AZ29)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:52" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="167"/>
+      <c r="A31" s="197"/>
       <c r="B31" s="50"/>
       <c r="C31" s="50"/>
       <c r="D31" s="50"/>
@@ -6122,10 +6839,10 @@
       <c r="AC31" s="50"/>
       <c r="AD31" s="50"/>
       <c r="AE31" s="50"/>
-      <c r="AF31" s="168"/>
-      <c r="AG31" s="165"/>
+      <c r="AF31" s="198"/>
+      <c r="AG31" s="195"/>
       <c r="AH31" s="9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="AN31" s="41"/>
       <c r="AO31" s="41"/>
@@ -6134,15 +6851,15 @@
       <c r="AR31" s="41"/>
       <c r="AS31" s="41"/>
       <c r="AT31" s="37"/>
-      <c r="AU31" s="182"/>
-      <c r="AV31" s="183"/>
-      <c r="AW31" s="183"/>
-      <c r="AX31" s="183"/>
-      <c r="AY31" s="184"/>
-      <c r="AZ31" s="187"/>
+      <c r="AU31" s="212"/>
+      <c r="AV31" s="213"/>
+      <c r="AW31" s="213"/>
+      <c r="AX31" s="213"/>
+      <c r="AY31" s="214"/>
+      <c r="AZ31" s="217"/>
     </row>
     <row r="32" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A32" s="166">
+      <c r="A32" s="196">
         <f t="shared" si="36"/>
         <v>44166</v>
       </c>
@@ -6270,7 +6987,7 @@
         <f t="shared" si="39"/>
         <v>5</v>
       </c>
-      <c r="AG32" s="165">
+      <c r="AG32" s="195">
         <f t="shared" ref="AG32" si="40">SUM(B33:AF33)</f>
         <v>0</v>
       </c>
@@ -6291,7 +7008,7 @@
       <c r="AU32" s="2"/>
     </row>
     <row r="33" spans="1:54" x14ac:dyDescent="0.2">
-      <c r="A33" s="167"/>
+      <c r="A33" s="197"/>
       <c r="B33" s="50"/>
       <c r="C33" s="50"/>
       <c r="D33" s="50"/>
@@ -6323,9 +7040,9 @@
       <c r="AD33" s="50"/>
       <c r="AE33" s="50"/>
       <c r="AF33" s="50"/>
-      <c r="AG33" s="165"/>
+      <c r="AG33" s="195"/>
       <c r="AH33" s="9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="AT33" s="37"/>
       <c r="AU33" s="2"/>
@@ -6346,7 +7063,7 @@
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
       <c r="O34" s="156" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="P34" s="156"/>
       <c r="Q34" s="156"/>
@@ -6408,7 +7125,7 @@
       <c r="AF35" s="159"/>
       <c r="AG35" s="155"/>
       <c r="AH35" s="13" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="AK35" s="68">
         <f>SUM(AK10:AK33)</f>
@@ -6428,7 +7145,7 @@
     </row>
     <row r="37" spans="1:54" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="151" t="s">
-        <v>57</v>
+        <v>126</v>
       </c>
       <c r="B37" s="152"/>
       <c r="C37" s="152"/>
@@ -6465,7 +7182,7 @@
     </row>
     <row r="38" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A38" s="112" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B38" s="113"/>
       <c r="C38" s="113"/>
@@ -6476,7 +7193,7 @@
       <c r="F38" s="114"/>
       <c r="G38" s="114"/>
       <c r="H38" s="113" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="I38" s="113"/>
       <c r="J38" s="113"/>
@@ -6484,7 +7201,7 @@
       <c r="L38" s="113"/>
       <c r="M38" s="115"/>
       <c r="N38" s="111" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="O38" s="111"/>
       <c r="P38" s="111"/>
@@ -6505,7 +7222,7 @@
       <c r="AB38" s="120"/>
       <c r="AC38" s="121"/>
       <c r="AD38" s="122" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="AE38" s="123"/>
       <c r="AF38" s="124"/>
@@ -6516,10 +7233,10 @@
     </row>
     <row r="39" spans="1:54" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="28" t="s">
-        <v>61</v>
+        <v>127</v>
       </c>
       <c r="B39" s="94" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C39" s="95"/>
       <c r="D39" s="95"/>
@@ -6539,7 +7256,7 @@
       <c r="P39" s="102"/>
       <c r="Q39" s="103"/>
       <c r="R39" s="88" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="S39" s="89"/>
       <c r="T39" s="90"/>
@@ -6550,7 +7267,7 @@
       <c r="V39" s="92"/>
       <c r="W39" s="93"/>
       <c r="X39" s="88" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="Y39" s="89"/>
       <c r="Z39" s="90"/>
@@ -6561,7 +7278,7 @@
       <c r="AB39" s="120"/>
       <c r="AC39" s="121"/>
       <c r="AD39" s="122" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="AE39" s="123"/>
       <c r="AF39" s="124"/>
@@ -6578,32 +7295,32 @@
       <c r="AS39"/>
       <c r="AT39"/>
       <c r="AU39" s="64" t="s">
+        <v>59</v>
+      </c>
+      <c r="AV39" s="64" t="s">
+        <v>60</v>
+      </c>
+      <c r="AW39" s="64" t="s">
+        <v>61</v>
+      </c>
+      <c r="AX39" s="64" t="s">
+        <v>62</v>
+      </c>
+      <c r="AY39" s="64" t="s">
+        <v>63</v>
+      </c>
+      <c r="AZ39" s="64" t="s">
+        <v>64</v>
+      </c>
+      <c r="BA39" s="64" t="s">
         <v>65</v>
-      </c>
-      <c r="AV39" s="64" t="s">
-        <v>66</v>
-      </c>
-      <c r="AW39" s="64" t="s">
-        <v>67</v>
-      </c>
-      <c r="AX39" s="64" t="s">
-        <v>68</v>
-      </c>
-      <c r="AY39" s="64" t="s">
-        <v>69</v>
-      </c>
-      <c r="AZ39" s="64" t="s">
-        <v>70</v>
-      </c>
-      <c r="BA39" s="64" t="s">
-        <v>71</v>
       </c>
       <c r="BB39"/>
     </row>
     <row r="40" spans="1:54" s="2" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="29"/>
       <c r="B40" s="94" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C40" s="95"/>
       <c r="D40" s="95"/>
@@ -6623,7 +7340,7 @@
       <c r="P40" s="105"/>
       <c r="Q40" s="106"/>
       <c r="R40" s="88" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="S40" s="89"/>
       <c r="T40" s="90"/>
@@ -6634,7 +7351,7 @@
       <c r="V40" s="92"/>
       <c r="W40" s="93"/>
       <c r="X40" s="88" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="Y40" s="89"/>
       <c r="Z40" s="90"/>
@@ -6645,7 +7362,7 @@
       <c r="AB40" s="120"/>
       <c r="AC40" s="121"/>
       <c r="AD40" s="122" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="AE40" s="123"/>
       <c r="AF40" s="124"/>
@@ -6660,10 +7377,10 @@
       <c r="AQ40" s="1"/>
       <c r="AR40" s="1"/>
       <c r="AS40" s="70" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="AT40" s="72" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="AU40" s="72">
         <v>1</v>
@@ -6685,7 +7402,7 @@
     <row r="41" spans="1:54" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="29"/>
       <c r="B41" s="94" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C41" s="95"/>
       <c r="D41" s="95"/>
@@ -6705,7 +7422,7 @@
       <c r="P41" s="105"/>
       <c r="Q41" s="106"/>
       <c r="R41" s="88" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="S41" s="89"/>
       <c r="T41" s="90"/>
@@ -6716,7 +7433,7 @@
       <c r="V41" s="92"/>
       <c r="W41" s="93"/>
       <c r="X41" s="88" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="Y41" s="89"/>
       <c r="Z41" s="90"/>
@@ -6727,7 +7444,7 @@
       <c r="AB41" s="120"/>
       <c r="AC41" s="121"/>
       <c r="AD41" s="122" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="AE41" s="123"/>
       <c r="AF41" s="124"/>
@@ -6735,10 +7452,10 @@
       <c r="AH41" s="21"/>
       <c r="AK41" s="37"/>
       <c r="AS41" s="70" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="AT41" s="74" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="AU41" s="73">
         <v>1</v>
@@ -6759,7 +7476,7 @@
     <row r="42" spans="1:54" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="29"/>
       <c r="B42" s="94" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C42" s="95"/>
       <c r="D42" s="95"/>
@@ -6775,12 +7492,12 @@
       <c r="N42" s="96"/>
       <c r="O42" s="97">
         <f>AZ30</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="P42" s="98"/>
       <c r="Q42" s="99"/>
       <c r="R42" s="88" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="S42" s="89"/>
       <c r="T42" s="90"/>
@@ -6791,18 +7508,18 @@
       <c r="V42" s="92"/>
       <c r="W42" s="93"/>
       <c r="X42" s="88" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="Y42" s="89"/>
       <c r="Z42" s="90"/>
       <c r="AA42" s="119">
         <f t="shared" si="42"/>
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="AB42" s="120"/>
       <c r="AC42" s="121"/>
       <c r="AD42" s="122" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="AE42" s="123"/>
       <c r="AF42" s="124"/>
@@ -6810,10 +7527,10 @@
       <c r="AH42" s="21"/>
       <c r="AK42" s="37"/>
       <c r="AS42" s="70" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="AT42" s="74" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="AU42" s="74"/>
       <c r="AV42" s="74">
@@ -6828,7 +7545,7 @@
     <row r="43" spans="1:54" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="30"/>
       <c r="B43" s="94" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C43" s="95"/>
       <c r="D43" s="95"/>
@@ -6848,7 +7565,7 @@
       <c r="P43" s="105"/>
       <c r="Q43" s="106"/>
       <c r="R43" s="88" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="S43" s="89"/>
       <c r="T43" s="90"/>
@@ -6859,7 +7576,7 @@
       <c r="V43" s="92"/>
       <c r="W43" s="93"/>
       <c r="X43" s="88" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="Y43" s="89"/>
       <c r="Z43" s="90"/>
@@ -6870,7 +7587,7 @@
       <c r="AB43" s="120"/>
       <c r="AC43" s="121"/>
       <c r="AD43" s="122" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="AE43" s="123"/>
       <c r="AF43" s="124"/>
@@ -6878,10 +7595,10 @@
       <c r="AH43" s="21"/>
       <c r="AK43" s="37"/>
       <c r="AS43" s="70" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="AT43" s="74" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="AU43" s="74"/>
       <c r="AV43" s="74"/>
@@ -6895,10 +7612,10 @@
     </row>
     <row r="44" spans="1:54" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="31" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B44" s="100" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C44" s="100"/>
       <c r="D44" s="100"/>
@@ -6926,12 +7643,12 @@
       <c r="Z44" s="100"/>
       <c r="AA44" s="144">
         <f>AA38-SUM(AA39:AC43)</f>
-        <v>1776</v>
+        <v>1768</v>
       </c>
       <c r="AB44" s="145"/>
       <c r="AC44" s="146"/>
       <c r="AD44" s="138" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="AE44" s="139"/>
       <c r="AF44" s="140"/>
@@ -6939,10 +7656,10 @@
       <c r="AH44" s="21"/>
       <c r="AK44" s="37"/>
       <c r="AS44" s="70" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="AT44" s="74" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="AU44" s="74"/>
       <c r="AV44" s="74"/>
@@ -6956,7 +7673,7 @@
     </row>
     <row r="45" spans="1:54" s="2" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="125" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B45" s="126"/>
       <c r="C45" s="126"/>
@@ -6981,19 +7698,18 @@
       <c r="V45" s="126"/>
       <c r="W45" s="127"/>
       <c r="X45" s="128">
-        <f>1/12*5</f>
-        <v>0.41666666666666663</v>
+        <v>1</v>
       </c>
       <c r="Y45" s="129"/>
       <c r="Z45" s="130"/>
       <c r="AA45" s="147">
         <f>AA44*X45</f>
-        <v>739.99999999999989</v>
+        <v>1768</v>
       </c>
       <c r="AB45" s="148"/>
       <c r="AC45" s="149"/>
       <c r="AD45" s="141" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="AE45" s="142"/>
       <c r="AF45" s="143"/>
@@ -7003,10 +7719,10 @@
       <c r="AJ45" s="23"/>
       <c r="AK45" s="37"/>
       <c r="AS45" s="70" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="AT45" s="74" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="AU45" s="74"/>
       <c r="AV45" s="74"/>
@@ -7064,10 +7780,10 @@
       <c r="AQ46" s="2"/>
       <c r="AR46" s="2"/>
       <c r="AS46" s="70" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="AT46" s="74" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="AU46" s="74"/>
       <c r="AV46" s="74"/>
@@ -7082,7 +7798,7 @@
     </row>
     <row r="47" spans="1:54" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="116" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B47" s="117"/>
       <c r="C47" s="117"/>
@@ -7107,10 +7823,10 @@
       <c r="V47" s="21"/>
       <c r="AK47" s="24"/>
       <c r="AS47" s="70" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="AT47" s="74" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="AU47" s="74"/>
       <c r="AV47" s="74">
@@ -7126,7 +7842,7 @@
     </row>
     <row r="48" spans="1:54" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="112" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
       <c r="B48" s="113"/>
       <c r="C48" s="113"/>
@@ -7148,7 +7864,7 @@
       <c r="P48" s="120"/>
       <c r="Q48" s="121"/>
       <c r="R48" s="122" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="S48" s="123"/>
       <c r="T48" s="124"/>
@@ -7163,10 +7879,10 @@
       <c r="AQ48" s="23"/>
       <c r="AR48" s="23"/>
       <c r="AS48" s="70" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="AT48" s="75" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="AU48" s="74"/>
       <c r="AV48" s="74"/>
@@ -7181,10 +7897,10 @@
     </row>
     <row r="49" spans="1:53" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="26" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B49" s="94" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C49" s="95"/>
       <c r="D49" s="95"/>
@@ -7200,12 +7916,12 @@
       <c r="N49" s="96"/>
       <c r="O49" s="131">
         <f>AA45</f>
-        <v>739.99999999999989</v>
+        <v>1768</v>
       </c>
       <c r="P49" s="132"/>
       <c r="Q49" s="133"/>
       <c r="R49" s="122" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="S49" s="123"/>
       <c r="T49" s="124"/>
@@ -7213,10 +7929,10 @@
       <c r="V49" s="21"/>
       <c r="AK49" s="37"/>
       <c r="AS49" s="70" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="AT49" s="74" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="AU49" s="75"/>
       <c r="AV49" s="75"/>
@@ -7232,10 +7948,10 @@
     </row>
     <row r="50" spans="1:53" s="2" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="27" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B50" s="134" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
       <c r="C50" s="134"/>
       <c r="D50" s="134"/>
@@ -7262,10 +7978,10 @@
       <c r="AH50" s="21"/>
       <c r="AK50" s="37"/>
       <c r="AS50" s="70" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="AT50" s="74" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="AU50" s="74"/>
       <c r="AV50" s="74"/>
@@ -7284,10 +8000,10 @@
       <c r="AH51" s="21"/>
       <c r="AK51" s="37"/>
       <c r="AS51" s="70" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="AT51" s="74" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="AU51" s="74"/>
       <c r="AV51" s="74"/>
@@ -7305,7 +8021,7 @@
     </row>
     <row r="52" spans="1:53" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="116" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B52" s="117"/>
       <c r="C52" s="117"/>
@@ -7330,10 +8046,10 @@
       <c r="AH52" s="21"/>
       <c r="AK52" s="37"/>
       <c r="AS52" s="70" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="AT52" s="74" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="AU52" s="74"/>
       <c r="AV52" s="74"/>
@@ -7353,7 +8069,7 @@
     </row>
     <row r="53" spans="1:53" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="112" t="s">
-        <v>109</v>
+        <v>130</v>
       </c>
       <c r="B53" s="113"/>
       <c r="C53" s="113"/>
@@ -7375,7 +8091,7 @@
       <c r="P53" s="120"/>
       <c r="Q53" s="121"/>
       <c r="R53" s="122" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="S53" s="123"/>
       <c r="T53" s="124"/>
@@ -7383,10 +8099,10 @@
       <c r="AH53" s="21"/>
       <c r="AK53" s="37"/>
       <c r="AS53" s="70" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="AT53" s="74" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="AU53" s="74">
         <v>1</v>
@@ -7402,7 +8118,7 @@
     </row>
     <row r="54" spans="1:53" s="2" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="85" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B54" s="86"/>
       <c r="C54" s="86"/>
@@ -7419,12 +8135,12 @@
       <c r="N54" s="87"/>
       <c r="O54" s="79">
         <f>X45*2080</f>
-        <v>866.66666666666663</v>
+        <v>2080</v>
       </c>
       <c r="P54" s="80"/>
       <c r="Q54" s="81"/>
       <c r="R54" s="82" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="S54" s="83"/>
       <c r="T54" s="84"/>
@@ -7432,10 +8148,10 @@
       <c r="AH54" s="21"/>
       <c r="AK54" s="37"/>
       <c r="AS54" s="70" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AT54" s="74" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="AU54" s="74"/>
       <c r="AV54" s="74"/>
@@ -7452,10 +8168,10 @@
       <c r="AH55" s="21"/>
       <c r="AK55" s="37"/>
       <c r="AS55" s="70" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="AT55" s="76" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="AU55" s="76"/>
       <c r="AV55" s="76"/>
@@ -7484,7 +8200,7 @@
       <c r="J56" s="33"/>
       <c r="K56" s="33"/>
       <c r="T56" s="110" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="U56" s="110"/>
       <c r="V56" s="110"/>
@@ -7545,7 +8261,7 @@
     </row>
     <row r="58" spans="1:53" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="107" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="B58" s="107"/>
       <c r="C58" s="107"/>
@@ -7558,7 +8274,7 @@
       <c r="J58" s="107"/>
       <c r="K58" s="107"/>
       <c r="Z58" s="107" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="AA58" s="107"/>
       <c r="AB58" s="107"/>
@@ -7599,7 +8315,7 @@
     </row>
     <row r="60" spans="1:53" s="2" customFormat="1" ht="24.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="150" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="B60" s="150"/>
       <c r="C60" s="150"/>
@@ -7644,7 +8360,7 @@
     </row>
     <row r="61" spans="1:53" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="150" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="B61" s="150"/>
       <c r="C61" s="150"/>
@@ -7689,7 +8405,7 @@
     </row>
     <row r="62" spans="1:53" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="150" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="B62" s="150"/>
       <c r="C62" s="150"/>
@@ -7734,7 +8450,7 @@
     </row>
     <row r="63" spans="1:53" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="150" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B63" s="150"/>
       <c r="C63" s="150"/>
@@ -7779,7 +8495,7 @@
     </row>
     <row r="64" spans="1:53" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="150" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="B64" s="150"/>
       <c r="C64" s="150"/>
@@ -7824,7 +8540,7 @@
     </row>
     <row r="65" spans="1:53" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="150" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B65" s="150"/>
       <c r="C65" s="150"/>
@@ -7869,7 +8585,7 @@
     </row>
     <row r="66" spans="1:53" s="2" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="150" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B66" s="150"/>
       <c r="C66" s="150"/>
@@ -7916,7 +8632,7 @@
     </row>
     <row r="67" spans="1:53" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="150" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B67" s="150"/>
       <c r="C67" s="150"/>
@@ -7973,7 +8689,7 @@
     </row>
     <row r="68" spans="1:53" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="150" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="B68" s="150"/>
       <c r="C68" s="150"/>
@@ -8019,7 +8735,7 @@
     </row>
     <row r="69" spans="1:53" s="2" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="150" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="B69" s="150"/>
       <c r="C69" s="150"/>
@@ -8068,7 +8784,7 @@
     </row>
     <row r="70" spans="1:53" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="150" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="B70" s="150"/>
       <c r="C70" s="150"/>
@@ -8118,7 +8834,7 @@
     </row>
     <row r="71" spans="1:53" s="2" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="150" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B71" s="150"/>
       <c r="C71" s="150"/>
@@ -8294,7 +9010,6 @@
       <c r="BA76" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="qHGQqVCDpAobJEUaN7ApBOxePmkuAi++wXK9w4qIcbpHmiB9Kl1V9q1W3NcTR0PAivoJvm9rd4fGbAGHLYc5Tg==" saltValue="S144Bjokf4DEz7x9bLejDQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="AT13:AZ29">
     <sortCondition ref="AW13:AW29"/>
   </sortState>
@@ -8653,15 +9368,12 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="81" fitToHeight="0" orientation="landscape" r:id="rId2"/>
-  <headerFooter>
-    <oddFooter>&amp;L&amp;F&amp;C&amp;D&amp;R&amp;P - &amp;N</oddFooter>
-  </headerFooter>
+  <pageSetup paperSize="9" scale="76" fitToHeight="0" orientation="landscape" r:id="rId2"/>
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="36" max="16383" man="1"/>
   </rowBreaks>
   <ignoredErrors>
-    <ignoredError sqref="AF30:AF31 AF26:AF27 AF20:AF21 AF16:AF17 AD12:AF12 B19:AF19 D11:AF11 B31 D17:F17 B13:F13 H13:AF13 H17:V17 B15:R15 T15:AF15 X17:AE17" unlockedFormula="1"/>
+    <ignoredError sqref="AF30:AF31 AF26:AF27 AF20:AF21 AF16:AF17 AD12:AF12 B19:AF19 C11:AF11 B31 D17:F17 B13:F13 H13:AF13 H17:V17 B15:R15 T15:AF15 X17:AE17" unlockedFormula="1"/>
     <ignoredError sqref="AW22:AX22" formula="1"/>
     <ignoredError sqref="AO14:AP14 AO25:AR29 AO24:AP24 AR24 AR14:AR23 AO16:AP23 AP15"/>
   </ignoredErrors>

</xml_diff>